<commit_message>
01042021 - Quasar All Atık
1- Geolocation
2- Başlangıç bitiş marker
</commit_message>
<xml_diff>
--- a/Denemeler/Harita/All Atik/all-atik-app/distance-matrix-response-converter/Distances.xlsx
+++ b/Denemeler/Harita/All Atik/all-atik-app/distance-matrix-response-converter/Distances.xlsx
@@ -1,35 +1,51 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{610820D1-EB18-420C-8CBD-62191B3F556E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Distances" state="visible" r:id="rId3"/>
+    <sheet name="Distances" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -37,14 +53,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -381,132 +419,180 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.5703125" style="1" customWidth="1"/>
+    <col min="2" max="7" width="6" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
         <v>0</v>
       </c>
-      <c r="B1">
+      <c r="C2" s="3">
         <v>1313</v>
       </c>
-      <c r="C1">
+      <c r="D2" s="3">
         <v>17476</v>
       </c>
-      <c r="D1">
+      <c r="E2" s="3">
         <v>4969</v>
       </c>
-      <c r="E1">
+      <c r="F2" s="3">
         <v>10670</v>
       </c>
-      <c r="F1">
+      <c r="G2" s="3">
         <v>10184</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="3" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
         <v>1044</v>
       </c>
-      <c r="B2">
+      <c r="C3" s="3">
         <v>0</v>
       </c>
-      <c r="C2">
+      <c r="D3" s="3">
         <v>17701</v>
       </c>
-      <c r="D2">
+      <c r="E3" s="3">
         <v>5194</v>
       </c>
-      <c r="E2">
+      <c r="F3" s="3">
         <v>10895</v>
       </c>
-      <c r="F2">
+      <c r="G3" s="3">
         <v>10409</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="4" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
         <v>17769</v>
       </c>
-      <c r="B3">
+      <c r="C4" s="3">
         <v>16672</v>
       </c>
-      <c r="C3">
+      <c r="D4" s="3">
         <v>0</v>
       </c>
-      <c r="D3">
+      <c r="E4" s="3">
         <v>13411</v>
       </c>
-      <c r="E3">
+      <c r="F4" s="3">
         <v>9887</v>
       </c>
-      <c r="F3">
+      <c r="G4" s="3">
         <v>10649</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="5" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
         <v>4163</v>
       </c>
-      <c r="B4">
+      <c r="C5" s="3">
         <v>5028</v>
       </c>
-      <c r="C4">
+      <c r="D5" s="3">
         <v>14059</v>
       </c>
-      <c r="D4">
+      <c r="E5" s="3">
         <v>0</v>
       </c>
-      <c r="E4">
+      <c r="F5" s="3">
         <v>7672</v>
       </c>
-      <c r="F4">
+      <c r="G5" s="3">
         <v>7630</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="6" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
         <v>12093</v>
       </c>
-      <c r="B5">
+      <c r="C6" s="3">
         <v>11297</v>
       </c>
-      <c r="C5">
+      <c r="D6" s="3">
         <v>10140</v>
       </c>
-      <c r="D5">
+      <c r="E6" s="3">
         <v>6983</v>
       </c>
-      <c r="E5">
+      <c r="F6" s="3">
         <v>0</v>
       </c>
-      <c r="F5">
+      <c r="G6" s="3">
         <v>1388</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="7" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
         <v>11785</v>
       </c>
-      <c r="B6">
+      <c r="C7" s="3">
         <v>10989</v>
       </c>
-      <c r="C6">
+      <c r="D7" s="3">
         <v>13556</v>
       </c>
-      <c r="D6">
+      <c r="E7" s="3">
         <v>7179</v>
       </c>
-      <c r="E6">
+      <c r="F7" s="3">
         <v>1826</v>
       </c>
-      <c r="F6">
+      <c r="G7" s="3">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>